<commit_message>
version 2.0 production analysis
</commit_message>
<xml_diff>
--- a/data/processed/prod_per_day.xlsx
+++ b/data/processed/prod_per_day.xlsx
@@ -1,21 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Notas de Estudio\Proyectos\production_analysis__project\production_analysis\data\processed\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A81CCCC4-676C-4EE9-8A42-FFAD70D3327C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A670FB4-ACBD-400B-AFBE-64C5E063E577}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -52,6 +62,9 @@
     <t>EB G4</t>
   </si>
   <si>
+    <t>EB-017</t>
+  </si>
+  <si>
     <t>EB-026</t>
   </si>
   <si>
@@ -212,9 +225,6 @@
   </si>
   <si>
     <t>EB-125</t>
-  </si>
-  <si>
-    <t>EB-17</t>
   </si>
   <si>
     <t>EB-18</t>
@@ -582,9 +592,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61:D62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -605,13 +622,13 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>27474.398000000001</v>
+        <v>26976.736000000001</v>
       </c>
       <c r="C2">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2">
-        <v>981</v>
+        <v>1038</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -619,13 +636,13 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>196686.935</v>
+        <v>195265.00599999999</v>
       </c>
       <c r="C3">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3">
-        <v>7285</v>
+        <v>6974</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -633,13 +650,13 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>8089.308</v>
+        <v>7180.0919999999996</v>
       </c>
       <c r="C4">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D4">
-        <v>506</v>
+        <v>552</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -647,13 +664,13 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>16388.185000000001</v>
+        <v>9642.6820000000007</v>
       </c>
       <c r="C5">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="D5">
-        <v>683</v>
+        <v>567</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -661,13 +678,13 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>9600.7240000000002</v>
+        <v>15270.753000000001</v>
       </c>
       <c r="C6">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="D6">
-        <v>565</v>
+        <v>636</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -675,13 +692,13 @@
         <v>9</v>
       </c>
       <c r="B7">
-        <v>13153.621999999999</v>
+        <v>17781.901999999998</v>
       </c>
       <c r="C7">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D7">
-        <v>692</v>
+        <v>635</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -689,10 +706,13 @@
         <v>10</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>15478.249</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>2211</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -700,13 +720,10 @@
         <v>11</v>
       </c>
       <c r="B9">
-        <v>1514.2660000000001</v>
+        <v>0</v>
       </c>
       <c r="C9">
-        <v>7</v>
-      </c>
-      <c r="D9">
-        <v>216</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -714,13 +731,10 @@
         <v>12</v>
       </c>
       <c r="B10">
-        <v>5182.6239999999998</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <v>22</v>
-      </c>
-      <c r="D10">
-        <v>236</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -728,13 +742,13 @@
         <v>13</v>
       </c>
       <c r="B11">
-        <v>5697.268</v>
+        <v>7543.6379999999999</v>
       </c>
       <c r="C11">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D11">
-        <v>259</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -742,10 +756,13 @@
         <v>14</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>8331.7960000000003</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>29</v>
+      </c>
+      <c r="D12">
+        <v>287</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -819,13 +836,10 @@
         <v>21</v>
       </c>
       <c r="B19">
-        <v>5724.9539999999997</v>
+        <v>0</v>
       </c>
       <c r="C19">
-        <v>22</v>
-      </c>
-      <c r="D19">
-        <v>260</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -833,13 +847,13 @@
         <v>22</v>
       </c>
       <c r="B20">
-        <v>5797.15</v>
+        <v>8902.3060000000005</v>
       </c>
       <c r="C20">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D20">
-        <v>264</v>
+        <v>307</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -847,13 +861,13 @@
         <v>23</v>
       </c>
       <c r="B21">
-        <v>5379.2439999999997</v>
+        <v>7775.5919999999996</v>
       </c>
       <c r="C21">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D21">
-        <v>245</v>
+        <v>268</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -861,13 +875,13 @@
         <v>24</v>
       </c>
       <c r="B22">
-        <v>23369.965</v>
+        <v>6278.4809999999998</v>
       </c>
       <c r="C22">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D22">
-        <v>806</v>
+        <v>224</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -875,13 +889,13 @@
         <v>25</v>
       </c>
       <c r="B23">
-        <v>19263.987000000001</v>
+        <v>24505.077000000001</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="D23">
-        <v>771</v>
+        <v>817</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -889,10 +903,13 @@
         <v>26</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>20381.385999999999</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <v>755</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -922,13 +939,10 @@
         <v>29</v>
       </c>
       <c r="B27">
-        <v>7928.98</v>
+        <v>0</v>
       </c>
       <c r="C27">
-        <v>13</v>
-      </c>
-      <c r="D27">
-        <v>610</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -936,13 +950,13 @@
         <v>30</v>
       </c>
       <c r="B28">
-        <v>3913.84</v>
+        <v>6384.3739999999998</v>
       </c>
       <c r="C28">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="D28">
-        <v>652</v>
+        <v>532</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -950,10 +964,13 @@
         <v>31</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>19447.400000000001</v>
       </c>
       <c r="C29">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <v>720</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -961,13 +978,10 @@
         <v>32</v>
       </c>
       <c r="B30">
-        <v>4436.3959999999997</v>
+        <v>0</v>
       </c>
       <c r="C30">
-        <v>25</v>
-      </c>
-      <c r="D30">
-        <v>177</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -975,13 +989,13 @@
         <v>33</v>
       </c>
       <c r="B31">
-        <v>4501.424</v>
+        <v>3746.7849999999999</v>
       </c>
       <c r="C31">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D31">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -989,13 +1003,13 @@
         <v>34</v>
       </c>
       <c r="B32">
-        <v>2324.71</v>
+        <v>2909.549</v>
       </c>
       <c r="C32">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D32">
-        <v>122</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1003,10 +1017,13 @@
         <v>35</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>2939.634</v>
       </c>
       <c r="C33">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="D33">
+        <v>173</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1014,10 +1031,13 @@
         <v>36</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>4500.17</v>
       </c>
       <c r="C34">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D34">
+        <v>250</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1069,13 +1089,10 @@
         <v>41</v>
       </c>
       <c r="B39">
-        <v>3949.1190000000001</v>
+        <v>0</v>
       </c>
       <c r="C39">
-        <v>23</v>
-      </c>
-      <c r="D39">
-        <v>172</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1083,13 +1100,13 @@
         <v>42</v>
       </c>
       <c r="B40">
-        <v>3032.0720000000001</v>
+        <v>4272.3010000000004</v>
       </c>
       <c r="C40">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="D40">
-        <v>144</v>
+        <v>225</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -1097,13 +1114,13 @@
         <v>43</v>
       </c>
       <c r="B41">
-        <v>4080.5309999999999</v>
+        <v>3609.3919999999998</v>
       </c>
       <c r="C41">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>163</v>
+        <v>201</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -1111,13 +1128,13 @@
         <v>44</v>
       </c>
       <c r="B42">
-        <v>4661.4160000000002</v>
+        <v>3000.3910000000001</v>
       </c>
       <c r="C42">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D42">
-        <v>194</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -1125,13 +1142,13 @@
         <v>45</v>
       </c>
       <c r="B43">
-        <v>4428.0839999999998</v>
+        <v>5408.902</v>
       </c>
       <c r="C43">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D43">
-        <v>185</v>
+        <v>216</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -1139,13 +1156,13 @@
         <v>46</v>
       </c>
       <c r="B44">
-        <v>4138.9070000000002</v>
+        <v>5136.067</v>
       </c>
       <c r="C44">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D44">
-        <v>166</v>
+        <v>223</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -1153,13 +1170,13 @@
         <v>47</v>
       </c>
       <c r="B45">
-        <v>4920.0870000000004</v>
+        <v>3263.3919999999998</v>
       </c>
       <c r="C45">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D45">
-        <v>224</v>
+        <v>155</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -1167,13 +1184,13 @@
         <v>48</v>
       </c>
       <c r="B46">
-        <v>4960.2730000000001</v>
+        <v>1962.914</v>
       </c>
       <c r="C46">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D46">
-        <v>207</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -1181,13 +1198,13 @@
         <v>49</v>
       </c>
       <c r="B47">
-        <v>4961.4750000000004</v>
+        <v>4427.9889999999996</v>
       </c>
       <c r="C47">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D47">
-        <v>236</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -1195,10 +1212,13 @@
         <v>50</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>3616.8049999999998</v>
       </c>
       <c r="C48">
-        <v>0</v>
+        <v>18</v>
+      </c>
+      <c r="D48">
+        <v>201</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,10 +1226,13 @@
         <v>51</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>1934.93</v>
       </c>
       <c r="C49">
-        <v>0</v>
+        <v>9</v>
+      </c>
+      <c r="D49">
+        <v>215</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -1217,10 +1240,13 @@
         <v>52</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>8988.9950000000008</v>
       </c>
       <c r="C50">
-        <v>0</v>
+        <v>17</v>
+      </c>
+      <c r="D50">
+        <v>529</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -1228,10 +1254,13 @@
         <v>53</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>7050.8710000000001</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>11</v>
+      </c>
+      <c r="D51">
+        <v>641</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1239,10 +1268,13 @@
         <v>54</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>7174.3860000000004</v>
       </c>
       <c r="C52">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D52">
+        <v>512</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -1250,10 +1282,13 @@
         <v>55</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>10210.671</v>
       </c>
       <c r="C53">
-        <v>0</v>
+        <v>21</v>
+      </c>
+      <c r="D53">
+        <v>486</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -1261,10 +1296,13 @@
         <v>56</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>6634.0780000000004</v>
       </c>
       <c r="C54">
-        <v>0</v>
+        <v>14</v>
+      </c>
+      <c r="D54">
+        <v>474</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -1272,13 +1310,10 @@
         <v>57</v>
       </c>
       <c r="B55">
-        <v>22677.46</v>
+        <v>0</v>
       </c>
       <c r="C55">
-        <v>29</v>
-      </c>
-      <c r="D55">
-        <v>782</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -1286,13 +1321,13 @@
         <v>58</v>
       </c>
       <c r="B56">
-        <v>21998.476999999999</v>
+        <v>22164.903999999999</v>
       </c>
       <c r="C56">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D56">
-        <v>815</v>
+        <v>739</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -1300,13 +1335,13 @@
         <v>59</v>
       </c>
       <c r="B57">
-        <v>24347.998</v>
+        <v>15979.769</v>
       </c>
       <c r="C57">
         <v>24</v>
       </c>
       <c r="D57">
-        <v>1014</v>
+        <v>666</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -1314,13 +1349,13 @@
         <v>60</v>
       </c>
       <c r="B58">
-        <v>16829.601999999999</v>
+        <v>32662.631000000001</v>
       </c>
       <c r="C58">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D58">
-        <v>647</v>
+        <v>1126</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -1328,13 +1363,13 @@
         <v>61</v>
       </c>
       <c r="B59">
-        <v>8230.7720000000008</v>
+        <v>5900.9470000000001</v>
       </c>
       <c r="C59">
-        <v>26</v>
+        <v>13</v>
       </c>
       <c r="D59">
-        <v>317</v>
+        <v>454</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -1342,13 +1377,13 @@
         <v>62</v>
       </c>
       <c r="B60">
-        <v>117087.96</v>
+        <v>7664.6989999999996</v>
       </c>
       <c r="C60">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D60">
-        <v>5576</v>
+        <v>319</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -1356,13 +1391,13 @@
         <v>63</v>
       </c>
       <c r="B61">
-        <v>134001.71200000009</v>
+        <v>167190.272</v>
       </c>
       <c r="C61">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D61">
-        <v>4621</v>
+        <v>5573</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,13 +1405,13 @@
         <v>64</v>
       </c>
       <c r="B62">
-        <v>59381.760000000002</v>
+        <v>79586.593000000008</v>
       </c>
       <c r="C62">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D62">
-        <v>2474</v>
+        <v>5306</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>